<commit_message>
new expert result KI
</commit_message>
<xml_diff>
--- a/03-30cow_GS_label_expert_response/results/GS_label_submission_track_master.xlsx
+++ b/03-30cow_GS_label_expert_response/results/GS_label_submission_track_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/03-30cow_GS_label_expert_response/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{F1D378CC-E7F6-D04B-9DEF-7DD515FBB73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A9F943-E2DA-604A-B5AB-07C7805CE849}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{F1D378CC-E7F6-D04B-9DEF-7DD515FBB73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04FE3245-C37E-B143-877E-D88A8FFB3B9A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>SB</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>Nov-11-2023</t>
+  </si>
+  <si>
+    <t>all_submitted_trackerNov-11-2023.csv</t>
   </si>
 </sst>
 </file>
@@ -559,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,6 +928,20 @@
         <v>30</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>